<commit_message>
add d13C unc nosams
</commit_message>
<xml_diff>
--- a/data_raw/Summary_metadata/Carbonate_isotopes_BA3A_NSHQ14.xlsx
+++ b/data_raw/Summary_metadata/Carbonate_isotopes_BA3A_NSHQ14.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melo.d/Desktop/Research/thesis_prep/manuscripts/Oman-14CH4/Oman-14CH4/data_raw/Summary_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC57AEDB-2F52-F44E-A730-323DA640C2B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE2CE81-A001-4E4E-9055-1135E6DC8D06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="11320" windowWidth="37340" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="44">
   <si>
     <t>NSHQ14</t>
   </si>
@@ -1564,10 +1564,10 @@
   <dimension ref="A1:X10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T6" sqref="T6"/>
+      <selection pane="bottomRight" activeCell="U2" sqref="U2:U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1731,8 +1731,8 @@
       <c r="T2" s="7">
         <v>-14.99</v>
       </c>
-      <c r="U2" s="7" t="s">
-        <v>1</v>
+      <c r="U2" s="7">
+        <v>0.1</v>
       </c>
       <c r="V2" s="7" t="s">
         <v>1</v>
@@ -1805,8 +1805,8 @@
       <c r="T3" s="7">
         <v>-7.67</v>
       </c>
-      <c r="U3" s="7" t="s">
-        <v>1</v>
+      <c r="U3" s="7">
+        <v>0.1</v>
       </c>
       <c r="V3" s="7" t="s">
         <v>1</v>
@@ -1879,8 +1879,8 @@
       <c r="T4" s="7">
         <v>-8.56</v>
       </c>
-      <c r="U4" s="7" t="s">
-        <v>1</v>
+      <c r="U4" s="7">
+        <v>0.1</v>
       </c>
       <c r="V4" s="7" t="s">
         <v>1</v>
@@ -1953,8 +1953,8 @@
       <c r="T5" s="19">
         <v>-9.74</v>
       </c>
-      <c r="U5" s="7" t="s">
-        <v>1</v>
+      <c r="U5" s="7">
+        <v>0.1</v>
       </c>
       <c r="V5" s="7" t="s">
         <v>1</v>
@@ -2027,8 +2027,8 @@
       <c r="T6" s="19">
         <v>-9.6199999999999992</v>
       </c>
-      <c r="U6" s="7" t="s">
-        <v>1</v>
+      <c r="U6" s="7">
+        <v>0.1</v>
       </c>
       <c r="V6" s="7" t="s">
         <v>1</v>
@@ -2101,8 +2101,8 @@
       <c r="T7" s="19">
         <v>-12.92</v>
       </c>
-      <c r="U7" s="7" t="s">
-        <v>1</v>
+      <c r="U7" s="7">
+        <v>0.1</v>
       </c>
       <c r="V7" s="7" t="s">
         <v>1</v>

</xml_diff>